<commit_message>
Added more messaging, included more default calibration scales
</commit_message>
<xml_diff>
--- a/data/data_selection/data_selection.xlsx
+++ b/data/data_selection/data_selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B31A25-C29F-CF4C-AA27-A3D535FD6B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7564175-ECE2-3446-AB2E-CD06F3645D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23000" yWindow="3940" windowWidth="27240" windowHeight="16440" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
+    <workbookView xWindow="2880" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E2A43AB0-C9B5-4349-922D-876081C672EC}</author>
+    <author>tc={E74B7E44-2395-6C42-B73D-2EC1F22A60C7}</author>
   </authors>
   <commentList>
     <comment ref="E9" authorId="0" shapeId="0" xr:uid="{E2A43AB0-C9B5-4349-922D-876081C672EC}">
@@ -49,12 +50,20 @@
     I just made these CH4 dates up for testing</t>
       </text>
     </comment>
+    <comment ref="C11" authorId="1" shapeId="0" xr:uid="{E74B7E44-2395-6C42-B73D-2EC1F22A60C7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check these</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -114,9 +123,6 @@
   </si>
   <si>
     <t># NOTE: ENSURE CELLS ARE FORMATTED AS TEXT, NOT DATES. IF PASTING VALUES ENSURE YOU "MATCH DESTINATION FORMATTING" TO PREVENT EXCEL FROM CONVERTING TO DATE AND TIME</t>
-  </si>
-  <si>
-    <t>1978-01-01 00:00</t>
   </si>
   <si>
     <t>Picarro start</t>
@@ -150,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +171,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -514,6 +526,9 @@
   <threadedComment ref="E9" dT="2023-07-22T05:26:38.42" personId="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" id="{E2A43AB0-C9B5-4349-922D-876081C672EC}">
     <text>I just made these CH4 dates up for testing</text>
   </threadedComment>
+  <threadedComment ref="C11" dT="2023-07-26T20:04:11.42" personId="{34B736E8-4CAD-3843-A1A8-25F59C5B220F}" id="{E74B7E44-2395-6C42-B73D-2EC1F22A60C7}">
+    <text>Check these</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -522,7 +537,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +560,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -560,7 +575,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -608,15 +623,15 @@
         <v>13</v>
       </c>
       <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -625,33 +640,33 @@
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
@@ -686,13 +701,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>

</xml_diff>